<commit_message>
feat: nip gurus and pwa
</commit_message>
<xml_diff>
--- a/public/assets/import/contoh_format_import_guru.xlsx
+++ b/public/assets/import/contoh_format_import_guru.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1zaru\Downloads\Documents\Contoh Format Sipapii\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ngoding\sipapii\public\assets\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1228C5E9-4B0D-4F2E-89C5-EF24EB486A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4742A3B4-6299-424D-BDC2-DBC2FB2126D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34680" yWindow="3975" windowWidth="17280" windowHeight="9075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>no</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>0812332123</t>
+  </si>
+  <si>
+    <t>nip</t>
+  </si>
+  <si>
+    <t>11233211123122</t>
   </si>
 </sst>
 </file>
@@ -75,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -358,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -370,25 +377,31 @@
     <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>